<commit_message>
Update to use DOLA 2020 dataset, issue #13.
</commit_message>
<xml_diff>
--- a/workflow/BaselineScenario/00-Synopsis/scenario-config.xlsx
+++ b/workflow/BaselineScenario/00-Synopsis/scenario-config.xlsx
@@ -683,7 +683,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -755,7 +755,7 @@
       <c r="E10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F10" t="str">
+      <c r="F10" s="12" t="str">
         <f>ScenarioId</f>
         <v>Baseline</v>
       </c>
@@ -773,7 +773,7 @@
       <c r="E11" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F11" t="str">
+      <c r="F11" s="12" t="str">
         <f>ScenarioDescription</f>
         <v>Baseline with basic status quo assumptions and estimates.</v>
       </c>
@@ -791,7 +791,7 @@
       <c r="E12" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F12" t="str">
+      <c r="F12" s="12" t="str">
         <f>ScenarioFolder</f>
         <v>BaselineScenario</v>
       </c>
@@ -809,7 +809,7 @@
       <c r="E13" s="9">
         <v>1980</v>
       </c>
-      <c r="F13" t="str">
+      <c r="F13" s="12" t="str">
         <f>TEXT(StartYear,"0000")</f>
         <v>1980</v>
       </c>
@@ -827,7 +827,7 @@
       <c r="E14" s="9">
         <v>2050</v>
       </c>
-      <c r="F14" t="str">
+      <c r="F14" s="12" t="str">
         <f>TEXT(EndYear,"0000")</f>
         <v>2050</v>
       </c>
@@ -846,7 +846,7 @@
         <f>StartYear</f>
         <v>1980</v>
       </c>
-      <c r="F15" t="str">
+      <c r="F15" s="12" t="str">
         <f>TEXT(HistStartYear,"0000")</f>
         <v>1980</v>
       </c>
@@ -862,11 +862,11 @@
         <v>21</v>
       </c>
       <c r="E16" s="4">
-        <v>2018</v>
-      </c>
-      <c r="F16" t="str">
+        <v>2019</v>
+      </c>
+      <c r="F16" s="12" t="str">
         <f>TEXT(HistEndYear,"0000")</f>
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>49</v>
@@ -881,11 +881,11 @@
       </c>
       <c r="E17" s="12">
         <f>HistEndYear + 1</f>
-        <v>2019</v>
-      </c>
-      <c r="F17" t="str">
+        <v>2020</v>
+      </c>
+      <c r="F17" s="12" t="str">
         <f>TEXT(ForecastStartYear,"0000")</f>
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>48</v>
@@ -902,7 +902,7 @@
         <f>EndYear</f>
         <v>2050</v>
       </c>
-      <c r="F18" t="str">
+      <c r="F18" s="12" t="str">
         <f>TEXT(ForecastEndYear,"0000")</f>
         <v>2050</v>
       </c>

</xml_diff>